<commit_message>
Move checks and variable creation to other liss repo. Put background variable documentation in separate table.
</commit_message>
<xml_diff>
--- a/utilities/dashboard/background_var_description.xlsx
+++ b/utilities/dashboard/background_var_description.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Background Variables</t>
   </si>
   <si>
-    <t xml:space="preserve">educ</t>
+    <t xml:space="preserve">educ_group</t>
   </si>
   <si>
     <t xml:space="preserve">Education Level</t>
@@ -58,10 +58,10 @@
     <t xml:space="preserve">Education</t>
   </si>
   <si>
-    <t xml:space="preserve">our_inc_group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Income Tercile</t>
+    <t xml:space="preserve">income_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income Group</t>
   </si>
   <si>
     <t xml:space="preserve">Income</t>
@@ -94,6 +94,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -115,6 +116,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,12 +190,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="21.95"/>

</xml_diff>

<commit_message>
Move to have different background variables for each tab.
</commit_message>
<xml_diff>
--- a/utilities/dashboard/background_var_description.xlsx
+++ b/utilities/dashboard/background_var_description.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t xml:space="preserve">new_name</t>
   </si>
@@ -31,12 +31,12 @@
     <t xml:space="preserve">nice_name_english</t>
   </si>
   <si>
+    <t xml:space="preserve">topic_english</t>
+  </si>
+  <si>
     <t xml:space="preserve">group_english</t>
   </si>
   <si>
-    <t xml:space="preserve">topic_english</t>
-  </si>
-  <si>
     <t xml:space="preserve">age_group</t>
   </si>
   <si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Background Variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background Overview</t>
   </si>
   <si>
     <t xml:space="preserve">educ_group</t>
@@ -187,10 +190,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -199,7 +202,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="6" style="0" width="14.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -218,6 +222,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -233,75 +238,75 @@
         <v>8</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First move towards creating the correlation tab data.
</commit_message>
<xml_diff>
--- a/utilities/dashboard/background_var_description.xlsx
+++ b/utilities/dashboard/background_var_description.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t xml:space="preserve">new_name</t>
   </si>
@@ -83,6 +83,21 @@
   </si>
   <si>
     <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_bin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fine Grained Age Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background Correlation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sector</t>
   </si>
 </sst>
 </file>
@@ -190,16 +205,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ6"/>
+  <dimension ref="A1:AMJ8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="6" style="0" width="14.39"/>
@@ -307,6 +322,40 @@
       </c>
       <c r="E6" s="0" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restructure in preparation for the correlation plot.
</commit_message>
<xml_diff>
--- a/utilities/dashboard/background_var_description.xlsx
+++ b/utilities/dashboard/background_var_description.xlsx
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Gender</t>
   </si>
   <si>
-    <t xml:space="preserve">age_bin</t>
+    <t xml:space="preserve">age_bins</t>
   </si>
   <si>
     <t xml:space="preserve">Fine Grained Age Group</t>
@@ -208,13 +208,13 @@
   <dimension ref="A1:AMJ8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="6" style="0" width="14.39"/>

</xml_diff>

<commit_message>
Add bottom text. Work on tables.
</commit_message>
<xml_diff>
--- a/utilities/dashboard/background_var_description.xlsx
+++ b/utilities/dashboard/background_var_description.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t xml:space="preserve">new_name</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t xml:space="preserve">Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_mental_health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mental Health Before</t>
   </si>
 </sst>
 </file>
@@ -205,10 +211,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -237,7 +243,6 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -356,6 +361,23 @@
       </c>
       <c r="E8" s="0" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove several groups and rename others.
</commit_message>
<xml_diff>
--- a/utilities/dashboard/background_var_description.xlsx
+++ b/utilities/dashboard/background_var_description.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Background Overview</t>
   </si>
   <si>
-    <t xml:space="preserve">educ_group</t>
+    <t xml:space="preserve">edu</t>
   </si>
   <si>
     <t xml:space="preserve">Education Level</t>
@@ -214,7 +214,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fix labels and restructure from_data_to_dashboard.
</commit_message>
<xml_diff>
--- a/utilities/dashboard/background_var_description.xlsx
+++ b/utilities/dashboard/background_var_description.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t xml:space="preserve">new_name</t>
   </si>
@@ -85,6 +85,15 @@
     <t xml:space="preserve">Gender</t>
   </si>
   <si>
+    <t xml:space="preserve">base_mental_health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mental Health Before</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mental Health</t>
+  </si>
+  <si>
     <t xml:space="preserve">age_bins</t>
   </si>
   <si>
@@ -98,12 +107,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">base_mental_health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mental Health Before</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -138,6 +141,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF21409A"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -185,12 +195,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -203,6 +217,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF21409A"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -214,12 +288,12 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="21.95"/>
@@ -337,47 +411,47 @@
         <v>22</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="0" t="s">
+    </row>
+    <row r="9" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>9</v>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major update on the captions and labels of the groups and background variables.
</commit_message>
<xml_diff>
--- a/utilities/dashboard/background_var_description.xlsx
+++ b/utilities/dashboard/background_var_description.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Background Overview</t>
   </si>
   <si>
-    <t xml:space="preserve">Respondents are categorized into groups of those younger than 40, those between 40 and 65 and those above 65. There are approximately 1600 people younger than 40 in the sample. 2300 respondents are between 40 to 65 years old and 1600 are older than 65.</t>
+    <t xml:space="preserve">Responses are shown by age group. There are approximately 1600 people younger than 40 in the sample. 2300 respondents are between 40 to 65 years old and 1600 are older than 65.</t>
   </si>
   <si>
     <t xml:space="preserve">edu</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Education</t>
   </si>
   <si>
-    <t xml:space="preserve">Respondents are categorized by their level of schooling. There are approximately 2000 respondents who have a high school diploma or less, 1300 respondents attended junior college, 1400 went to college and 700 went to university.</t>
+    <t xml:space="preserve">Responses are shown for people with different levels of schooling. There are approximately 2000 respondents who have a high school diploma or less, 1300 respondents attended junior college, 1400 went to college and 700 went to university.</t>
   </si>
   <si>
     <t xml:space="preserve">income_group</t>
@@ -67,7 +67,12 @@
     <t xml:space="preserve">Income</t>
   </si>
   <si>
-    <t xml:space="preserve">Respondents are categorized by the household’s net income adjusting for household composition. You can think of it as the net income available to an adult in the household. We account for children and that it’s cheaper when there are more people in a household. There are four groups with approx. 1200 respondents each: those earning less than 2500 Euros per month and adult, those earning between 2500 and 4500 Euros, those between 4500 and 7500 and those earning more than 7500 per month and adult.</t>
+    <t xml:space="preserve">Responses are split according to the respondents’ households’ net income adjusting for household composition. 
+You can think of it as the net income available to an adult in the household. 
+We account for children and that living costs are lower when there are more people in a household. 
+There are four groups with approx. 1200 respondents each: 
+those earning less than 2500 Euros per month and adult, those earning between 2500 and 4500 Euros, 
+Those between 4500 and 7500 and those earning more than 7500 per month and adult.</t>
   </si>
   <si>
     <t xml:space="preserve">health_group</t>
@@ -76,7 +81,7 @@
     <t xml:space="preserve">Health</t>
   </si>
   <si>
-    <t xml:space="preserve">Respondents are categorized by how they rated their own health in 2018. Approximately 800 rated their health as “moderate or less”, 2600 as “good” and 1200 rated their health as “excellent”.</t>
+    <t xml:space="preserve">Responses are shown for people with different self-reported health in 2018. Approximately 800 rated their health as “moderate or less”, 2600 as “good” and 1200 rated their health as “excellent”.</t>
   </si>
   <si>
     <t xml:space="preserve">gender</t>
@@ -85,7 +90,7 @@
     <t xml:space="preserve">Gender</t>
   </si>
   <si>
-    <t xml:space="preserve">Among the approximately 5500 respondents, 3000 were women and 2500 were men.</t>
+    <t xml:space="preserve">Responses are shown for men and women separately. Among the approximately 5500 respondents 3000 were women and 2500 were men.</t>
   </si>
 </sst>
 </file>
@@ -204,7 +209,7 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -235,7 +240,7 @@
       </c>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
@@ -252,7 +257,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
@@ -269,7 +274,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
@@ -303,7 +308,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Add an aggregated scatter plot (#8)
* Add bottom text. Work on tables.

* Add color column to group_info

* Remove several groups and rename others.

* Implement new color scheme, make get_colors more flexible.

* Fix labels and restructure from_data_to_dashboard.

* Put data description for dashboard under version control.

* Add number of observations to hovertools in barplot and stacked barplot.

* Bin variables whose distributions were not very visible.

* Refactor barplot code.

* Use adult equivalent approach by OECD to calculate income groups.

* Nice and dynamic background variable documentation.

* Move to directory structure for bokeh serve. 

* Major update on the captions and labels of the groups and background variables.

* Add IZA static and templates folder for nice layout.

Co-authored-by: Janos Gabler <janos.gabler@gmail.com>
</commit_message>
<xml_diff>
--- a/utilities/dashboard/background_var_description.xlsx
+++ b/utilities/dashboard/background_var_description.xlsx
@@ -20,29 +20,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t xml:space="preserve">new_name</t>
   </si>
   <si>
+    <t xml:space="preserve">nice_name_english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">topic_english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group_english</t>
+  </si>
+  <si>
     <t xml:space="preserve">label_english</t>
   </si>
   <si>
-    <t xml:space="preserve">nice_name_english</t>
-  </si>
-  <si>
-    <t xml:space="preserve">topic_english</t>
-  </si>
-  <si>
-    <t xml:space="preserve">group_english</t>
-  </si>
-  <si>
     <t xml:space="preserve">age_group</t>
   </si>
   <si>
-    <t xml:space="preserve">Age Group</t>
-  </si>
-  <si>
     <t xml:space="preserve">Age</t>
   </si>
   <si>
@@ -52,37 +49,48 @@
     <t xml:space="preserve">Background Overview</t>
   </si>
   <si>
-    <t xml:space="preserve">educ_group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Education Level</t>
+    <t xml:space="preserve">Responses are shown by age group. There are approximately 1600 people younger than 40 in the sample. 2300 respondents are between 40 to 65 years old and 1600 are older than 65.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edu</t>
   </si>
   <si>
     <t xml:space="preserve">Education</t>
   </si>
   <si>
+    <t xml:space="preserve">Responses are shown for people with different levels of schooling. There are approximately 2000 respondents who have a high school diploma or less, 1300 respondents attended junior college, 1400 went to college and 700 went to university.</t>
+  </si>
+  <si>
     <t xml:space="preserve">income_group</t>
   </si>
   <si>
-    <t xml:space="preserve">Income Group</t>
-  </si>
-  <si>
     <t xml:space="preserve">Income</t>
   </si>
   <si>
+    <t xml:space="preserve">Responses are split according to the respondents’ households’ net income adjusting for household composition. 
+You can think of it as the net income available to an adult in the household. 
+We account for children and that living costs are lower when there are more people in a household. 
+There are four groups with approx. 1200 respondents each: 
+those earning less than 2500 Euros per month and adult, those earning between 2500 and 4500 Euros, 
+Those between 4500 and 7500 and those earning more than 7500 per month and adult.</t>
+  </si>
+  <si>
     <t xml:space="preserve">health_group</t>
   </si>
   <si>
-    <t xml:space="preserve">Health Status</t>
-  </si>
-  <si>
     <t xml:space="preserve">Health</t>
   </si>
   <si>
+    <t xml:space="preserve">Responses are shown for people with different self-reported health in 2018. Approximately 800 rated their health as “moderate or less”, 2600 as “good” and 1200 rated their health as “excellent”.</t>
+  </si>
+  <si>
     <t xml:space="preserve">gender</t>
   </si>
   <si>
     <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responses are shown for men and women separately. Among the approximately 5500 respondents 3000 were women and 2500 were men.</t>
   </si>
 </sst>
 </file>
@@ -164,13 +172,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -193,38 +209,38 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="6" style="0" width="14.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="6.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="6" style="0" width="14.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
@@ -237,11 +253,11 @@
       <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>10</v>
       </c>
@@ -249,16 +265,16 @@
         <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
@@ -266,16 +282,16 @@
         <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>16</v>
       </c>
@@ -283,16 +299,16 @@
         <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>19</v>
       </c>
@@ -300,13 +316,13 @@
         <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>9</v>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>